<commit_message>
Implemented auto PM trip planning & cost estimation
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-26.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-26.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,79 +43,43 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-26T06:23:54.029Z</t>
+    <t>2025-11-26T20:06:07.721Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"377e3016-aab0-4571-b2fe-86c23066f14f","EventDtm":"2025-11-26T06:19:10Z","AppDtm":"2025-11-26T06:19:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:19:10Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":15.479479,"GPSLongitude":73.969728,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T06:19:10Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":28.82,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":149.28,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.95,"AmpPhB":10.1,"AmpPhC":10.95,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.92,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":87.66,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.95,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.52,"TRtn1Q":null,"TRtn2":5.54,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.32,"PctSucVlvQ":null,"TSup1":4.93,"TSup1Q":null,"TSup2":4.95,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:23:54.064Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7d0f6bc2-ef73-4ce7-9a3b-fcaec9c62d5d","EventDtm":"2025-11-26T06:20:00Z","AppDtm":"2025-11-26T06:20:18Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:20:00Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":9,"GPSLastLock":0,"GPSLatitude":19.252891,"GPSLongitude":73.016492,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":28.8,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:23:54.076Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5df690e3-c988-4cfa-a976-9cc567914bfe","EventDtm":"2025-11-26T06:20:38Z","AppDtm":"2025-11-26T06:20:56Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:20:38Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.547773,"GPSLongitude":78.380489,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.3,"BatteryVoltage":8.1,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:23:54.083Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"da09b026-d1e9-4f2b-bed7-bf8ae52b61e4","EventDtm":"2025-11-26T06:21:24Z","AppDtm":"2025-11-26T06:21:42Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:21:24Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.533223,"GPSLongitude":78.433006,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":"-53","ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8.1,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T06:21:24Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":29.5,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":250,"PSucQ":"asProvided","TDis":60.4,"TDisQ":null,"FreqComp":null,"TSuc":22.5,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":880,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":16.14,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":417.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"On","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.88,"TRtn1Q":null,"TRtn2":136.4,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":null,"TSup1":5.31,"TSup1Q":null,"TSup2":5.3,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:23:54.092Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"346f2372-6f7c-4b3b-ad27-1642ab900d2e","EventDtm":"2025-11-26T06:22:38Z","AppDtm":"2025-11-26T06:22:52Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:22:38Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":26.606096,"GPSLongitude":80.723681,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":false,"ExtPowerVoltage":7.4,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:30:55.125Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e532d4a3-e5b2-49ae-8a12-ee34c25cf343","EventDtm":"2025-11-26T06:23:57Z","AppDtm":"2025-11-26T06:24:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:23:57Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.516213,"GPSLongitude":82.962446,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957964","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.7,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T06:23:57Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":30,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":70,"PSucQ":"asProvided","TDis":80.9,"TDisQ":null,"FreqComp":null,"TSuc":-10.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":890,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":51,"PctExpVlvQ":null,"TEvap":22,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":388.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.7,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.59,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:30:55.252Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ab192f4f-f7c0-4d98-ad7f-452ccf8c6411","EventDtm":"2025-11-26T06:24:09Z","AppDtm":"2025-11-26T06:24:26Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:24:09Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":12.805018,"GPSLongitude":77.662177,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T06:24:09Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":96.75,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.34,"AmpPhB":10.88,"AmpPhC":11.34,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.02,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.08,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.78,"TRtn1Q":null,"TRtn2":5.79,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.45,"PctSucVlvQ":null,"TSup1":5.09,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:30:55.255Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d741fc33-787e-432a-9d9c-fc9ebd6d1ee0","EventDtm":"2025-11-26T06:24:48Z","AppDtm":"2025-11-26T06:25:05Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:24:48Z","DeviceID":"JSGA623040329","GPSLockState":"LOCKED","GPSSatelliteCount":8,"GPSLastLock":0,"GPSLatitude":17.547979,"GPSLongitude":78.380757,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:30:55.257Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"55aea18d-368d-49db-bedf-3ee528427d83","EventDtm":"2025-11-26T06:24:46Z","AppDtm":"2025-11-26T06:25:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:24:46Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.515942,"GPSLongitude":82.981169,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T06:24:46Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":29.72,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":135.61,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.46,"AmpPhB":11.06,"AmpPhC":11.46,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.03,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.11,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408.89,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.02,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.74,"TRtn1Q":null,"TRtn2":3.79,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":5.36,"PctSucVlvQ":null,"TSup1":2.97,"TSup1Q":null,"TSup2":3.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:30:55.259Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f9865f9d-ffa8-4490-bbed-b3f66812892c","EventDtm":"2025-11-26T08:08:00Z","AppDtm":"2025-11-26T06:26:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T08:08:00Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":5217,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":33.8,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:30:55.263Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"833f2347-12e0-4357-abda-7190da1df074","EventDtm":"2025-11-26T06:25:40Z","AppDtm":"2025-11-26T06:26:21Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:25:40Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.310603,"GPSLongitude":91.717549,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T06:25:40Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":28.5,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":75.3,"TDisQ":null,"FreqComp":null,"TSuc":-25.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":980,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":86,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":397.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":93.6,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-26T06:30:55.266Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"48ae452b-109c-4d14-a4a4-91018b6ce0ca","EventDtm":"2025-11-26T06:27:21Z","AppDtm":"2025-11-26T06:27:37Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T06:27:21Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.364698,"GPSLongitude":75.581337,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-83","ExtPower":true,"ExtPowerVoltage":33.7,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T06:27:21Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":21,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":36,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":5.7,"AmpPhB":6.4,"AmpPhC":6.5,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":16.9,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":388,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.2,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":5.4,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e96257f1-3a05-4a2f-9c4e-9dd7f68212d4","EventDtm":"2025-11-26T19:58:16Z","AppDtm":"2025-11-26T19:58:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T19:58:16Z","DeviceID":"JSGA622180044","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":147,"GPSLatitude":26.764466,"GPSLongitude":80.882968,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"54","LAC":"30917","CID":"234230120","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":32.9,"BatteryVoltage":8.1,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618581","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T19:58:16Z","AssetType":"Reefer","AssetID":"TRIU6618581","OEM":"CARRIER","TAmb":16.86,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":104.95,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04900648","AmpPhA":11.75,"AmpPhB":12.34,"AmpPhC":11.75,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-1.53,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.34,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":426.19,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-2.35,"TRtn1Q":null,"TRtn2":-2.38,"TRtn2Q":null,"TSet":-3,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":10.43,"PctSucVlvQ":null,"TSup1":-3.02,"TSup1Q":null,"TSup2":-2.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-02T11:27:53Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":60,"RCAlias":"AL60","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-26T20:06:07.796Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e7c568d3-aaad-49cf-ba88-7205b0f100b1","EventDtm":"2025-11-26T19:59:44Z","AppDtm":"2025-11-26T20:00:03Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T19:59:44Z","DeviceID":"JSGA623040321","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":12.816277,"GPSLongitude":77.68725,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9057","CID":"180498700","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":31.8,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6617250","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-26T20:06:07.831Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"83568cd2-b74c-42b6-bc65-4b36a010fcce","EventDtm":"2025-11-26T20:03:56Z","AppDtm":"2025-11-26T20:04:10Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T20:03:56Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":26.644384,"GPSLongitude":88.468068,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323842","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.7,"BatteryVoltage":8.1,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T20:03:56Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":18.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":77.2,"TDisQ":null,"FreqComp":null,"TSuc":-14.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":-0.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":423.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":0.81,"TRtn1Q":null,"TRtn2":1.6,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":17.99,"PctSucVlvQ":null,"TSup1":0.12,"TSup1Q":null,"TSup2":1.8,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-26T20:06:08.393Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"925e9264-9281-4fb6-8fdb-2d25a0bbc0ef","EventDtm":"2025-11-26T20:04:16Z","AppDtm":"2025-11-26T20:04:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T20:04:16Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":26.606132,"GPSLongitude":80.723723,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193710","RSSI":"-79","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8,"DeviceTemp":14,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-26T20:06:08.953Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5805fde2-4ad1-4c70-ae25-620c91b315cf","EventDtm":"2025-11-26T20:04:33Z","AppDtm":"2025-11-26T20:04:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T20:04:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":12.805029,"GPSLongitude":77.662178,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T20:04:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":28.31,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":149.42,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":10.18,"AmpPhB":11.1,"AmpPhC":10.18,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.06,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.63,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.11,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.61,"TRtn1Q":null,"TRtn2":5.63,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.75,"PctSucVlvQ":null,"TSup1":5.09,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-26T20:07:04.694Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ba8e354d-f391-48d1-b488-e8709d49fc2c","EventDtm":"2025-11-26T20:06:47Z","AppDtm":"2025-11-26T20:07:04Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-26T20:06:47Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":16.824892,"GPSLongitude":78.131558,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-26T20:06:47Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":20.62,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":57.6,"TDisQ":null,"FreqComp":null,"TSuc":-28.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":395.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":4.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":9.45,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":16,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
   </si>
 </sst>
 </file>
@@ -504,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -747,198 +711,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>